<commit_message>
Report about to complete
</commit_message>
<xml_diff>
--- a/12. December-2019.xlsx
+++ b/12. December-2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="15260" windowHeight="7940"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="15260" windowHeight="7940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="6" r:id="rId1"/>
@@ -4868,7 +4868,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -23699,7 +23699,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -24445,8 +24445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView view="pageLayout" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25321,7 +25321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M203"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
@@ -32309,8 +32309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M179"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34918,7 +34918,7 @@
     <mergeCell ref="A56:F56"/>
   </mergeCells>
   <pageMargins left="1.43" right="0.7" top="0.79" bottom="0.28999999999999998" header="0.7" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>